<commit_message>
Imported final (?) images and fixed font size
Stuck on fixing scramble dots now
</commit_message>
<xml_diff>
--- a/linguistic_parameters/o1_corr.xlsx
+++ b/linguistic_parameters/o1_corr.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -40,16 +40,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>